<commit_message>
Add description column to field documentation
</commit_message>
<xml_diff>
--- a/querymodule/doc/API field lists.xlsx
+++ b/querymodule/doc/API field lists.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="60" windowWidth="28800" windowHeight="16380" activeTab="8"/>
+    <workbookView xWindow="-45" yWindow="60" windowWidth="28800" windowHeight="16380" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="patent" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6533" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6534" uniqueCount="554">
   <si>
     <t>API Field Name</t>
   </si>
@@ -2289,8 +2289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="G136" sqref="G136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21250,7 +21250,7 @@
   <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21288,6 +21288,9 @@
       </c>
       <c r="I1" s="14" t="s">
         <v>230</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -30010,7 +30013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -35487,7 +35490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -36047,7 +36050,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -36064,7 +36067,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -36081,7 +36084,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -36183,7 +36186,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -36200,7 +36203,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>142</v>
       </c>
@@ -36251,7 +36254,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -36285,7 +36288,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -36302,7 +36305,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -36387,7 +36390,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -36404,7 +36407,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -36591,7 +36594,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -36744,7 +36747,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>53</v>
       </c>
@@ -36795,7 +36798,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Fix type in API field lists and regenerate documentation
</commit_message>
<xml_diff>
--- a/querymodule/doc/API field lists.xlsx
+++ b/querymodule/doc/API field lists.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="60" windowWidth="28800" windowHeight="16380" activeTab="6"/>
+    <workbookView xWindow="-45" yWindow="60" windowWidth="28800" windowHeight="16380" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="patent" sheetId="1" r:id="rId1"/>
@@ -1454,9 +1454,6 @@
     <t>Inventor's city on a patent</t>
   </si>
   <si>
-    <t>Inventor's country on a patnet</t>
-  </si>
-  <si>
     <t>Inventor's city on most recent patent</t>
   </si>
   <si>
@@ -1696,6 +1693,9 @@
   </si>
   <si>
     <t>http://www.uspto.gov/web/patents/classification/selectbynum.htm</t>
+  </si>
+  <si>
+    <t>Inventor's country on a patent</t>
   </si>
 </sst>
 </file>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="J61" s="32" t="str">
         <f>VLOOKUP(A61,Common!$A$2:$E$199,5, FALSE)</f>
-        <v>Inventor's country on a patnet</v>
+        <v>Inventor's country on a patent</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13822,7 +13822,7 @@
       </c>
       <c r="J35" s="32" t="str">
         <f>VLOOKUP(A35,Common!$A$2:$E$199,5, FALSE)</f>
-        <v>Inventor's country on a patnet</v>
+        <v>Inventor's country on a patent</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -18385,7 +18385,7 @@
       </c>
       <c r="J42" s="32" t="str">
         <f>VLOOKUP(A42,Common!$A$2:$E$199,5, FALSE)</f>
-        <v>Inventor's country on a patnet</v>
+        <v>Inventor's country on a patent</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -22767,7 +22767,7 @@
       </c>
       <c r="J42" s="32" t="str">
         <f>VLOOKUP(A42,Common!$A$2:$E$199,5, FALSE)</f>
-        <v>Inventor's country on a patnet</v>
+        <v>Inventor's country on a patent</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -27149,7 +27149,7 @@
       </c>
       <c r="J42" s="32" t="str">
         <f>VLOOKUP(A42,Common!$A$2:$E$199,5, FALSE)</f>
-        <v>Inventor's country on a patnet</v>
+        <v>Inventor's country on a patent</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -30013,8 +30013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35490,9 +35490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO218"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -35534,7 +35532,7 @@
         <v>327</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="120" x14ac:dyDescent="0.25">
@@ -35548,10 +35546,10 @@
         <v>325</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -35585,7 +35583,7 @@
         <v>329</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="120" x14ac:dyDescent="0.25">
@@ -35602,7 +35600,7 @@
         <v>330</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -35616,10 +35614,10 @@
         <v>325</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -35633,7 +35631,7 @@
         <v>325</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>460</v>
@@ -35650,10 +35648,10 @@
         <v>325</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -35667,7 +35665,7 @@
         <v>325</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>465</v>
@@ -35684,10 +35682,10 @@
         <v>325</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>516</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="75" x14ac:dyDescent="0.25">
@@ -35735,10 +35733,10 @@
         <v>325</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -35774,10 +35772,10 @@
         <v>325</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -35791,10 +35789,10 @@
         <v>325</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -35808,10 +35806,10 @@
         <v>325</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="E17" s="32" t="s">
         <v>544</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -35825,10 +35823,10 @@
         <v>325</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -35842,10 +35840,10 @@
         <v>325</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>473</v>
+        <v>553</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -35859,10 +35857,10 @@
         <v>325</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -35876,10 +35874,10 @@
         <v>325</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -35893,10 +35891,10 @@
         <v>325</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -35910,7 +35908,7 @@
         <v>325</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>399</v>
@@ -35927,10 +35925,10 @@
         <v>325</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -35944,10 +35942,10 @@
         <v>325</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
@@ -35961,7 +35959,7 @@
         <v>325</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E26" s="31" t="s">
         <v>379</v>
@@ -35993,7 +35991,7 @@
         <v>325</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E27" s="31" t="s">
         <v>398</v>
@@ -36010,10 +36008,10 @@
         <v>325</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -36027,10 +36025,10 @@
         <v>325</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -36044,10 +36042,10 @@
         <v>325</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="75" x14ac:dyDescent="0.25">
@@ -36061,7 +36059,7 @@
         <v>325</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>397</v>
@@ -36081,7 +36079,7 @@
         <v>346</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
@@ -36095,7 +36093,7 @@
         <v>325</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E33" s="31" t="s">
         <v>396</v>
@@ -36115,7 +36113,7 @@
         <v>327</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -36129,7 +36127,7 @@
         <v>325</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>394</v>
@@ -36146,7 +36144,7 @@
         <v>325</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>389</v>
@@ -36163,7 +36161,7 @@
         <v>325</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>388</v>
@@ -36180,7 +36178,7 @@
         <v>325</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>386</v>
@@ -36197,10 +36195,10 @@
         <v>325</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -36214,7 +36212,7 @@
         <v>325</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E40" s="20" t="s">
         <v>384</v>
@@ -36231,10 +36229,10 @@
         <v>325</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -36248,10 +36246,10 @@
         <v>325</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -36265,7 +36263,7 @@
         <v>324</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E43" s="30" t="s">
         <v>413</v>
@@ -36282,7 +36280,7 @@
         <v>324</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>412</v>
@@ -36299,7 +36297,7 @@
         <v>324</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E45" s="30" t="s">
         <v>407</v>
@@ -36316,7 +36314,7 @@
         <v>324</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E46" s="30" t="s">
         <v>408</v>
@@ -36333,7 +36331,7 @@
         <v>324</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E47" s="30" t="s">
         <v>409</v>
@@ -36350,7 +36348,7 @@
         <v>324</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E48" s="35" t="s">
         <v>410</v>
@@ -36367,7 +36365,7 @@
         <v>324</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E49" s="31" t="s">
         <v>378</v>
@@ -36384,7 +36382,7 @@
         <v>324</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E50" s="31" t="s">
         <v>380</v>
@@ -36401,7 +36399,7 @@
         <v>324</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E51" s="31" t="s">
         <v>381</v>
@@ -36418,7 +36416,7 @@
         <v>324</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E52" s="31" t="s">
         <v>382</v>
@@ -36438,7 +36436,7 @@
         <v>347</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -36455,7 +36453,7 @@
         <v>347</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -36472,7 +36470,7 @@
         <v>347</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -36489,7 +36487,7 @@
         <v>347</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -36540,7 +36538,7 @@
         <v>347</v>
       </c>
       <c r="E59" s="28" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -36557,7 +36555,7 @@
         <v>347</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -36574,7 +36572,7 @@
         <v>347</v>
       </c>
       <c r="E61" s="32" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -36591,7 +36589,7 @@
         <v>347</v>
       </c>
       <c r="E62" s="32" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -36625,7 +36623,7 @@
         <v>347</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
@@ -36676,7 +36674,7 @@
         <v>347</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
@@ -36826,7 +36824,7 @@
         <v>322</v>
       </c>
       <c r="E75" s="32" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
@@ -36860,7 +36858,7 @@
         <v>347</v>
       </c>
       <c r="E77" s="32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
@@ -36894,7 +36892,7 @@
         <v>347</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
@@ -36911,7 +36909,7 @@
         <v>347</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -36945,7 +36943,7 @@
         <v>347</v>
       </c>
       <c r="E82" s="32" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -36962,7 +36960,7 @@
         <v>347</v>
       </c>
       <c r="E83" s="32" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -36979,7 +36977,7 @@
         <v>347</v>
       </c>
       <c r="E84" s="32" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -36996,7 +36994,7 @@
         <v>347</v>
       </c>
       <c r="E85" s="32" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -37081,7 +37079,7 @@
         <v>347</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -37098,7 +37096,7 @@
         <v>347</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -37149,7 +37147,7 @@
         <v>347</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -37166,7 +37164,7 @@
         <v>347</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -37183,7 +37181,7 @@
         <v>347</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -37200,7 +37198,7 @@
         <v>347</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -37217,7 +37215,7 @@
         <v>347</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -37234,7 +37232,7 @@
         <v>347</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -37319,7 +37317,7 @@
         <v>347</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -37336,7 +37334,7 @@
         <v>347</v>
       </c>
       <c r="E105" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -37523,7 +37521,7 @@
         <v>347</v>
       </c>
       <c r="E116" s="32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -37540,7 +37538,7 @@
         <v>347</v>
       </c>
       <c r="E117" s="32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -37693,7 +37691,7 @@
         <v>347</v>
       </c>
       <c r="E126" s="32" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -37894,7 +37892,7 @@
         <v>347</v>
       </c>
       <c r="E138" s="32" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -37911,7 +37909,7 @@
         <v>347</v>
       </c>
       <c r="E139" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -37928,7 +37926,7 @@
         <v>347</v>
       </c>
       <c r="E140" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -37945,7 +37943,7 @@
         <v>347</v>
       </c>
       <c r="E141" s="32" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -37962,7 +37960,7 @@
         <v>347</v>
       </c>
       <c r="E142" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -38081,7 +38079,7 @@
         <v>347</v>
       </c>
       <c r="E149" s="32" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -38098,7 +38096,7 @@
         <v>347</v>
       </c>
       <c r="E150" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -38234,7 +38232,7 @@
         <v>347</v>
       </c>
       <c r="E158" s="32" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -38881,7 +38879,7 @@
         <v>347</v>
       </c>
       <c r="E194" s="32" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>